<commit_message>
Add load MMA script and move files
</commit_message>
<xml_diff>
--- a/TLGAnalyticTheory/data/MMAdata/TLG data.xlsx
+++ b/TLGAnalyticTheory/data/MMAdata/TLG data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7320" tabRatio="617"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="7320" tabRatio="617"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,38 +455,38 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -494,7 +494,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -888,27 +888,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.75" style="1"/>
-    <col min="4" max="4" width="34.875" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.25" customWidth="1"/>
-    <col min="11" max="11" width="12.625" customWidth="1"/>
-    <col min="14" max="14" width="14.5" customWidth="1"/>
-    <col min="15" max="15" width="17.75" customWidth="1"/>
-    <col min="16" max="16" width="17.125" customWidth="1"/>
-    <col min="17" max="17" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="34.90625" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" customWidth="1"/>
+    <col min="11" max="11" width="12.6328125" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" customWidth="1"/>
+    <col min="15" max="15" width="17.7265625" customWidth="1"/>
+    <col min="16" max="16" width="17.08984375" customWidth="1"/>
+    <col min="17" max="17" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:17">
       <c r="B1" s="1" t="s">
         <v>53</v>
       </c>
@@ -958,7 +958,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:17">
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
@@ -966,7 +966,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:17">
       <c r="B3" s="1" t="s">
         <v>72</v>
       </c>
@@ -974,7 +974,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:17">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -985,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:17">
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
@@ -996,7 +996,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:17">
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:17">
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:17">
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:17">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:17">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:17">
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:17">
       <c r="C12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:17">
       <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="N13" s="5"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:17">
       <c r="C14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:17">
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:17">
       <c r="C16" s="1" t="s">
         <v>38</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:16">
       <c r="C17" s="1" t="s">
         <v>43</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:16">
       <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="2:16" ht="95.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:16" ht="95.15" customHeight="1">
       <c r="C19" s="1" t="s">
         <v>43</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:16">
       <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:16">
       <c r="C21" s="1" t="s">
         <v>52</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:16">
       <c r="C22" s="1" t="s">
         <v>61</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:16">
       <c r="D23" t="s">
         <v>64</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:16">
       <c r="C24" s="1" t="s">
         <v>66</v>
       </c>
@@ -1582,11 +1582,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:16">
       <c r="C25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E25">
@@ -1621,13 +1621,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:16">
       <c r="M26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:16">
       <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:16">
       <c r="B28" s="1" t="s">
         <v>76</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:16">
       <c r="B29" s="1" t="s">
         <v>74</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:16">
       <c r="B30" s="1" t="s">
         <v>76</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:16">
       <c r="B31" s="1" t="s">
         <v>76</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:16">
       <c r="B32" s="1" t="s">
         <v>86</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:15">
       <c r="B33" s="1" t="s">
         <v>74</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:15">
       <c r="B34" s="1" t="s">
         <v>86</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:15">
       <c r="B35" s="1" t="s">
         <v>99</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:15">
       <c r="B36" s="1" t="s">
         <v>99</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:15">
       <c r="B37" s="1" t="s">
         <v>108</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:15">
       <c r="B38" s="13" t="s">
         <v>112</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:15">
       <c r="B39" s="13" t="s">
         <v>112</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:15">
       <c r="B40" s="13" t="s">
         <v>112</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="2:15" ht="108" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:15" ht="101.5">
       <c r="B41" s="13" t="s">
         <v>112</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="2:15" ht="108" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:15" ht="101.5">
       <c r="B42" s="13" t="s">
         <v>112</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:15">
       <c r="M43" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2350,7 +2350,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:15">
       <c r="M44" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2359,241 +2359,241 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:15">
       <c r="M45" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:15">
       <c r="M46" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:15">
       <c r="M47" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:15">
       <c r="M48" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="49" spans="13:13">
       <c r="M49" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="50" spans="13:13">
       <c r="M50" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="51" spans="13:13">
       <c r="M51" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="52" spans="13:13">
       <c r="M52" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="53" spans="13:13">
       <c r="M53" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="54" spans="13:13">
       <c r="M54" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="55" spans="13:13">
       <c r="M55" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="56" spans="13:13">
       <c r="M56" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="57" spans="13:13">
       <c r="M57" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="58" spans="13:13">
       <c r="M58" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="59" spans="13:13">
       <c r="M59" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="60" spans="13:13">
       <c r="M60" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="61" spans="13:13">
       <c r="M61" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="62" spans="13:13">
       <c r="M62" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="63" spans="13:13">
       <c r="M63" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="64" spans="13:13">
       <c r="M64" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="65" spans="13:13">
       <c r="M65" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="66" spans="13:13">
       <c r="M66" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="67" spans="13:13">
       <c r="M67" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="68" spans="13:13">
       <c r="M68" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="69" spans="13:13">
       <c r="M69" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="70" spans="13:13">
       <c r="M70" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="71" spans="13:13">
       <c r="M71" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="72" spans="13:13">
       <c r="M72" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="73" spans="13:13">
       <c r="M73" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="74" spans="13:13">
       <c r="M74" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="75" spans="13:13">
       <c r="M75" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="76" spans="13:13">
       <c r="M76" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="77" spans="13:13">
       <c r="M77" s="3">
         <f t="shared" ref="M77:M84" si="4">L77/3600</f>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="78" spans="13:13">
       <c r="M78" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="79" spans="13:13">
       <c r="M79" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="80" spans="13:13">
       <c r="M80" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="81" spans="13:13">
       <c r="M81" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="82" spans="13:13">
       <c r="M82" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="83" spans="13:13">
       <c r="M83" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="13:13" x14ac:dyDescent="0.15">
+    <row r="84" spans="13:13">
       <c r="M84" s="3">
         <f t="shared" si="4"/>
         <v>0</v>

</xml_diff>